<commit_message>
add lab12 (add bug-report)
</commit_message>
<xml_diff>
--- a/lab11/lab11.xlsx
+++ b/lab11/lab11.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FA79C3-0F85-F347-A055-15161046F612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F05AE8-ACC7-40D3-9AE3-D465518ABF1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="25600" windowHeight="20020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="816" windowWidth="25596" windowHeight="20016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-план" sheetId="5" r:id="rId1"/>
@@ -19,19 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Чек-лист + Дефекты'!$A$1:$D$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="164">
   <si>
     <t>New</t>
   </si>
@@ -509,6 +501,21 @@
   </si>
   <si>
     <t>Система готова для внедрения в продакш</t>
+  </si>
+  <si>
+    <t>Неверная ошибка при отправке неверных параметров на авторизацию</t>
+  </si>
+  <si>
+    <t>Банковская система</t>
+  </si>
+  <si>
+    <t>Handlers.go</t>
+  </si>
+  <si>
+    <t>Marsel Garipov</t>
+  </si>
+  <si>
+    <t>При отправке post-запроса с invalid payoad данными на localhost:8082/sessions должна приходить ошибка HTTP 400 Bad request. А приходит HTTP 422 Unprocessible entity.</t>
   </si>
 </sst>
 </file>
@@ -518,7 +525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +656,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1101,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1267,6 +1281,67 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1289,6 +1364,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1306,102 +1385,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1751,26 +1766,26 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="2"/>
-    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="44.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1640625" style="1"/>
-    <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="17.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
     <col min="9" max="9" width="26.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="27.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" style="1" customWidth="1"/>
-    <col min="12" max="44" width="9.1640625" style="1"/>
-    <col min="45" max="16384" width="9.1640625" style="2"/>
+    <col min="11" max="11" width="20.44140625" style="1" customWidth="1"/>
+    <col min="12" max="44" width="9.109375" style="1"/>
+    <col min="45" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:45" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -1784,7 +1799,7 @@
       <c r="I2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:45" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>10</v>
@@ -1793,7 +1808,7 @@
       <c r="I3" s="6"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
         <v>90</v>
@@ -1807,7 +1822,7 @@
       <c r="I4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1818,7 +1833,7 @@
       <c r="I5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
         <v>28</v>
@@ -1831,16 +1846,16 @@
       <c r="I6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:45" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
@@ -1875,7 +1890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="73" t="s">
         <v>96</v>
@@ -1900,11 +1915,11 @@
       <c r="J10" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="75"/>
+      <c r="K10" s="100"/>
       <c r="L10" s="15"/>
       <c r="AS10" s="1"/>
     </row>
-    <row r="11" spans="1:45" s="69" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" s="69" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="70"/>
       <c r="B11" s="73" t="s">
         <v>97</v>
@@ -1929,7 +1944,7 @@
       <c r="J11" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="K11" s="76"/>
+      <c r="K11" s="101"/>
       <c r="L11" s="15"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1965,7 +1980,7 @@
       <c r="AR11" s="1"/>
       <c r="AS11" s="1"/>
     </row>
-    <row r="12" spans="1:45" s="69" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" s="69" customFormat="1" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="70"/>
       <c r="B12" s="73" t="s">
         <v>98</v>
@@ -1990,7 +2005,7 @@
       <c r="J12" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="K12" s="76"/>
+      <c r="K12" s="101"/>
       <c r="L12" s="15"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2026,7 +2041,7 @@
       <c r="AR12" s="1"/>
       <c r="AS12" s="1"/>
     </row>
-    <row r="13" spans="1:45" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="73" t="s">
         <v>94</v>
@@ -2051,11 +2066,11 @@
       <c r="J13" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="K13" s="77"/>
+      <c r="K13" s="102"/>
       <c r="L13" s="15"/>
       <c r="AS13" s="1"/>
     </row>
-    <row r="14" spans="1:45" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>23</v>
       </c>
@@ -2073,7 +2088,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -2085,7 +2100,7 @@
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -2097,7 +2112,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -2109,14 +2124,14 @@
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="21"/>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -2128,7 +2143,7 @@
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -2140,7 +2155,7 @@
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -2152,7 +2167,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -2176,42 +2191,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
       <c r="D1" s="25" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
-      <c r="G1" s="82" t="s">
+      <c r="G1" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="83"/>
-      <c r="I1" s="84"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="80"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="109"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="105"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
       <c r="D2" s="26">
         <v>43955</v>
       </c>
@@ -2227,7 +2242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>99</v>
       </c>
@@ -2240,7 +2255,7 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="23"/>
       <c r="B4" s="23" t="s">
         <v>100</v>
@@ -2253,7 +2268,7 @@
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23" t="s">
@@ -2266,7 +2281,7 @@
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
@@ -2279,7 +2294,7 @@
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="23" t="s">
@@ -2292,7 +2307,7 @@
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23" t="s">
@@ -2307,7 +2322,7 @@
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="23" t="s">
         <v>101</v>
@@ -2320,7 +2335,7 @@
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="23" t="s">
         <v>102</v>
@@ -2333,18 +2348,18 @@
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="96"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>103</v>
       </c>
@@ -2357,7 +2372,7 @@
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="23"/>
       <c r="B13" s="23" t="s">
         <v>104</v>
@@ -2370,7 +2385,7 @@
       <c r="H13" s="24"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="23" t="s">
         <v>105</v>
@@ -2383,7 +2398,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
@@ -2396,7 +2411,7 @@
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23" t="s">
@@ -2409,7 +2424,7 @@
       <c r="H16" s="24"/>
       <c r="I16" s="24"/>
     </row>
-    <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23" t="s">
@@ -2422,7 +2437,7 @@
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23" t="s">
@@ -2435,7 +2450,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23" t="s">
@@ -2448,7 +2463,7 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23" t="s">
@@ -2461,7 +2476,7 @@
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>121</v>
       </c>
@@ -2469,7 +2484,7 @@
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="23" t="s">
         <v>112</v>
@@ -2477,7 +2492,7 @@
       <c r="C22" s="23"/>
       <c r="D22" s="27"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23" t="s">
@@ -2485,7 +2500,7 @@
       </c>
       <c r="D23" s="27"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23" t="s">
@@ -2493,7 +2508,7 @@
       </c>
       <c r="D24" s="27"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23" t="s">
@@ -2501,7 +2516,7 @@
       </c>
       <c r="D25" s="27"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="23" t="s">
         <v>115</v>
@@ -2509,7 +2524,7 @@
       <c r="C26" s="23"/>
       <c r="D26" s="27"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23" t="s">
@@ -2517,7 +2532,7 @@
       </c>
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23" t="s">
@@ -2525,7 +2540,7 @@
       </c>
       <c r="D28" s="27"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23" t="s">
@@ -2533,7 +2548,7 @@
       </c>
       <c r="D29" s="27"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="23" t="s">
@@ -2541,7 +2556,7 @@
       </c>
       <c r="D30" s="27"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="23" t="s">
         <v>118</v>
@@ -2549,7 +2564,7 @@
       <c r="C31" s="23"/>
       <c r="D31" s="27"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
       <c r="C32" s="23" t="s">
@@ -2557,7 +2572,7 @@
       </c>
       <c r="D32" s="27"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="23"/>
       <c r="B33" s="23"/>
       <c r="C33" s="23" t="s">
@@ -2584,19 +2599,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E29"/>
+    <sheetView topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
       <c r="B1" s="30" t="s">
         <v>29</v>
@@ -2615,12 +2630,12 @@
       </c>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="85"/>
-      <c r="B2" s="87" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="112"/>
+      <c r="B2" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="116" t="s">
         <v>123</v>
       </c>
       <c r="D2" s="36"/>
@@ -2631,10 +2646,10 @@
       <c r="G2" s="39"/>
       <c r="H2" s="40"/>
     </row>
-    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="90"/>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="113"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="117"/>
       <c r="D3" s="36"/>
       <c r="E3" s="37"/>
       <c r="F3" s="38" t="s">
@@ -2643,12 +2658,12 @@
       <c r="G3" s="41"/>
       <c r="H3" s="40"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="42"/>
       <c r="B4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="76" t="s">
         <v>125</v>
       </c>
       <c r="D4" s="32"/>
@@ -2661,7 +2676,7 @@
       </c>
       <c r="H4" s="35"/>
     </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
@@ -2671,7 +2686,7 @@
       <c r="G5" s="45"/>
       <c r="H5" s="45"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="B6" s="30" t="s">
         <v>36</v>
@@ -2685,7 +2700,7 @@
       <c r="G6" s="49"/>
       <c r="H6" s="47"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="50" t="s">
         <v>37</v>
@@ -2701,7 +2716,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
@@ -2711,7 +2726,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="44"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
@@ -2721,7 +2736,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="52">
         <f>COUNTA(A12:A26)</f>
         <v>5</v>
@@ -2750,37 +2765,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.2">
-      <c r="A11" s="111" t="s">
+    <row r="11" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="114" t="s">
+      <c r="G11" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="115" t="s">
+      <c r="H11" s="85" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="116">
+    <row r="12" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="86">
         <v>1</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="88" t="s">
         <v>132</v>
       </c>
       <c r="C12" s="72"/>
@@ -2790,8 +2805,8 @@
       <c r="G12" s="72"/>
       <c r="H12" s="72"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="117">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="87">
         <v>2</v>
       </c>
       <c r="B13" s="23" t="s">
@@ -2810,8 +2825,8 @@
       </c>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="117">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="87">
         <v>3</v>
       </c>
       <c r="B14" s="23" t="s">
@@ -2830,8 +2845,8 @@
       </c>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="117">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="87">
         <v>4</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -2850,8 +2865,8 @@
       </c>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="117">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="87">
         <v>5</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -2870,89 +2885,89 @@
       </c>
       <c r="H16" s="23"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="99"/>
-      <c r="E19" s="100"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C20" s="105" t="s">
+      <c r="D19" s="118"/>
+      <c r="E19" s="119"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="103" t="s">
+      <c r="D20" s="120" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="104"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C21" s="105" t="s">
+      <c r="E20" s="121"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="103" t="s">
+      <c r="D21" s="120" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="104"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="121"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C22" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="101"/>
-      <c r="E22" s="102"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C23" s="105"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="110"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="122"/>
+      <c r="E22" s="123"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="77"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="80"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C24" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="109"/>
-      <c r="E24" s="110"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C25" s="105" t="s">
+      <c r="D24" s="79"/>
+      <c r="E24" s="80"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="109" t="s">
+      <c r="D25" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="110"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C26" s="105" t="s">
+      <c r="E25" s="80"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D26" s="109" t="s">
+      <c r="D26" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="E26" s="110"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="80"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="109"/>
-      <c r="E27" s="110"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="105" t="s">
+      <c r="D27" s="79"/>
+      <c r="E27" s="80"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="109" t="s">
+      <c r="D28" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="110"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C29" s="105" t="s">
+      <c r="E28" s="80"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="77" t="s">
         <v>127</v>
       </c>
       <c r="D29" s="23" t="s">
@@ -2960,25 +2975,25 @@
       </c>
       <c r="E29" s="23"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="107"/>
-      <c r="E30" s="107"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C31" s="24"/>
-      <c r="D31" s="107"/>
-      <c r="E31" s="107"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="110"/>
+      <c r="E31" s="110"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="24"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="107"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="110"/>
+      <c r="E32" s="110"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="24"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="108"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3007,15 +3022,15 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
       <c r="B1" s="30" t="s">
         <v>29</v>
@@ -3034,12 +3049,12 @@
       </c>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="85"/>
-      <c r="B2" s="87" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="112"/>
+      <c r="B2" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="116" t="s">
         <v>88</v>
       </c>
       <c r="D2" s="36"/>
@@ -3050,10 +3065,10 @@
       <c r="G2" s="39"/>
       <c r="H2" s="40"/>
     </row>
-    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="90"/>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="113"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="117"/>
       <c r="D3" s="36"/>
       <c r="E3" s="37"/>
       <c r="F3" s="38" t="s">
@@ -3062,12 +3077,12 @@
       <c r="G3" s="41"/>
       <c r="H3" s="40"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="42"/>
       <c r="B4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="76" t="s">
         <v>125</v>
       </c>
       <c r="D4" s="32"/>
@@ -3080,7 +3095,7 @@
       </c>
       <c r="H4" s="35"/>
     </row>
-    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
@@ -3090,7 +3105,7 @@
       <c r="G5" s="45"/>
       <c r="H5" s="45"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="B6" s="30" t="s">
         <v>36</v>
@@ -3104,7 +3119,7 @@
       <c r="G6" s="49"/>
       <c r="H6" s="47"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="50" t="s">
         <v>37</v>
@@ -3120,7 +3135,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="45"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
@@ -3130,7 +3145,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="44"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
@@ -3140,7 +3155,7 @@
       <c r="G9" s="45"/>
       <c r="H9" s="45"/>
     </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="52">
         <f>COUNTA(A12:A28)</f>
         <v>5</v>
@@ -3171,222 +3186,229 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.2">
-      <c r="A11" s="111" t="s">
+    <row r="11" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="114" t="s">
+      <c r="G11" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="115" t="s">
+      <c r="H11" s="85" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="120">
+    <row r="12" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="90">
         <v>1</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="126" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="118"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="88"/>
       <c r="H12" s="72"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="120">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="90">
         <v>2</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="88" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="118" t="s">
+      <c r="C13" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="124" t="s">
+      <c r="D13" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119"/>
-      <c r="G13" s="118" t="s">
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="88" t="s">
         <v>143</v>
       </c>
       <c r="H13" s="72"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="120">
+    <row r="14" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="90">
         <v>3</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="118" t="s">
+      <c r="C14" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D14" s="124" t="s">
+      <c r="D14" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="118" t="s">
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="88" t="s">
         <v>145</v>
       </c>
       <c r="H14" s="72"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="120">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="90">
         <v>4</v>
       </c>
-      <c r="B15" s="118" t="s">
+      <c r="B15" s="88" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="88" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="124" t="s">
+      <c r="D15" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="118" t="s">
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="88" t="s">
         <v>136</v>
       </c>
       <c r="H15" s="72"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="123">
+    <row r="16" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="93">
         <v>5</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="118" t="s">
+      <c r="C16" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="125" t="s">
+      <c r="D16" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="121"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="118" t="s">
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="88" t="s">
         <v>145</v>
       </c>
       <c r="H16" s="23"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="131" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C20" s="105" t="s">
+      <c r="D19" s="126"/>
+      <c r="E19" s="126"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="127" t="s">
+      <c r="D20" s="124" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="127"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C21" s="105" t="s">
+      <c r="E20" s="124"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="77" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="127" t="s">
+      <c r="D21" s="124" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="127"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C22" s="105" t="s">
+      <c r="E21" s="124"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="127" t="s">
+      <c r="D22" s="124" t="s">
         <v>150</v>
       </c>
-      <c r="E22" s="127"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C23" s="105" t="s">
+      <c r="E22" s="124"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="D23" s="127" t="s">
+      <c r="D23" s="124" t="s">
         <v>152</v>
       </c>
-      <c r="E23" s="127"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C24" s="105" t="s">
+      <c r="E23" s="124"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="77" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="129" t="s">
+      <c r="D24" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="129"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C25" s="105" t="s">
+      <c r="E24" s="125"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="103" t="s">
+      <c r="D25" s="120" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="104"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="121"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C26" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="101"/>
-      <c r="E26" s="102"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C27" s="105"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="102"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="130" t="s">
+      <c r="D26" s="122"/>
+      <c r="E26" s="123"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="77"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="123"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="101"/>
-      <c r="E28" s="102"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C29" s="128" t="s">
+      <c r="D28" s="122"/>
+      <c r="E28" s="123"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="97" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="101" t="s">
+      <c r="D29" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="102"/>
+      <c r="E29" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
@@ -3394,13 +3416,6 @@
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -3414,55 +3429,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="25.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="127" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="128"/>
+      <c r="D1" s="129"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="60"/>
+      <c r="B2" s="60">
+        <v>1</v>
+      </c>
       <c r="C2" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="61"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>160</v>
+      </c>
       <c r="C3" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="23"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="23" t="s">
+        <v>67</v>
+      </c>
       <c r="C4" s="59" t="s">
         <v>56</v>
       </c>
       <c r="D4" s="23"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="23" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" s="59" t="s">
         <v>58</v>
       </c>
@@ -3470,7 +3499,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="62" t="s">
         <v>59</v>
       </c>
@@ -3482,7 +3511,7 @@
       </c>
       <c r="D6" s="23"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="62" t="s">
         <v>7</v>
       </c>
@@ -3494,7 +3523,7 @@
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="62" t="s">
         <v>63</v>
       </c>
@@ -3506,7 +3535,7 @@
       </c>
       <c r="D8" s="23"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="62" t="s">
         <v>6</v>
       </c>
@@ -3516,7 +3545,7 @@
       </c>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="62" t="s">
         <v>8</v>
       </c>
@@ -3526,7 +3555,7 @@
       </c>
       <c r="D10" s="23"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="59" t="s">
         <v>68</v>
       </c>
@@ -3534,23 +3563,27 @@
       <c r="C11" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="23"/>
-    </row>
-    <row r="12" spans="1:4" ht="188.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D11" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-    </row>
-    <row r="13" spans="1:4" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="131" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="132"/>
+      <c r="D12" s="132"/>
+    </row>
+    <row r="13" spans="1:4" ht="145.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3578,22 +3611,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35.77734375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="64" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -3601,7 +3634,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -3609,7 +3642,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -3617,7 +3650,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>74</v>
       </c>
@@ -3626,7 +3659,7 @@
       </c>
       <c r="C7" s="23"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>75</v>
       </c>
@@ -3637,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>76</v>
       </c>
@@ -3648,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>77</v>
       </c>
@@ -3659,7 +3692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>78</v>
       </c>
@@ -3667,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>79</v>
       </c>
@@ -3675,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>80</v>
       </c>
@@ -3683,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>81</v>
       </c>
@@ -3691,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>82</v>
       </c>
@@ -3699,7 +3732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>83</v>
       </c>
@@ -3707,12 +3740,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="64" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>158</v>
       </c>

</xml_diff>